<commit_message>
Fixed fractions bug where undo/reset did not work properly
</commit_message>
<xml_diff>
--- a/src/images/Fractions.xlsx
+++ b/src/images/Fractions.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="106">
   <si>
     <t>+</t>
   </si>
@@ -91,9 +91,6 @@
   </si>
   <si>
     <t>7/10</t>
-  </si>
-  <si>
-    <t>14/33</t>
   </si>
   <si>
     <t>1/12</t>
@@ -680,8 +677,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H99"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A77" workbookViewId="0">
-      <selection activeCell="E99" sqref="E99"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -849,7 +846,7 @@
         <v>10</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>0</v>
@@ -858,7 +855,7 @@
         <v>12</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>25</v>
+        <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -866,13 +863,13 @@
         <v>11</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>18</v>
@@ -892,7 +889,7 @@
         <v>19</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -900,13 +897,13 @@
         <v>13</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>3</v>
@@ -923,10 +920,10 @@
         <v>0</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
@@ -934,13 +931,13 @@
         <v>15</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>12</v>
@@ -951,7 +948,7 @@
         <v>16</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>0</v>
@@ -960,7 +957,7 @@
         <v>13</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -994,7 +991,7 @@
         <v>3</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1002,7 +999,7 @@
         <v>19</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" s="3" t="s">
         <v>0</v>
@@ -1019,16 +1016,16 @@
         <v>20</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D20" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="E20" s="3" t="s">
         <v>37</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1036,16 +1033,16 @@
         <v>21</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1053,16 +1050,16 @@
         <v>22</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C22" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1070,16 +1067,16 @@
         <v>23</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C23" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1087,16 +1084,16 @@
         <v>24</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C24" s="3" t="s">
         <v>0</v>
       </c>
       <c r="D24" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E24" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="E24" s="3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1110,10 +1107,10 @@
         <v>0</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1121,16 +1118,16 @@
         <v>26</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E26" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1141,7 +1138,7 @@
         <v>2</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>18</v>
@@ -1155,16 +1152,16 @@
         <v>28</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D28" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1175,7 +1172,7 @@
         <v>14</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>18</v>
@@ -1189,10 +1186,10 @@
         <v>30</v>
       </c>
       <c r="B30" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D30" s="3" t="s">
         <v>4</v>
@@ -1206,13 +1203,13 @@
         <v>31</v>
       </c>
       <c r="B31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>44</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>18</v>
@@ -1223,16 +1220,16 @@
         <v>32</v>
       </c>
       <c r="B32" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C32" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D32" s="3" t="s">
         <v>7</v>
       </c>
       <c r="E32" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1243,13 +1240,13 @@
         <v>10</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E33" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1260,13 +1257,13 @@
         <v>10</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>22</v>
       </c>
       <c r="E34" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1277,13 +1274,13 @@
         <v>10</v>
       </c>
       <c r="C35" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D35" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="D35" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="E35" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1294,13 +1291,13 @@
         <v>14</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D36" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -1311,13 +1308,13 @@
         <v>13</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D37" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1328,13 +1325,13 @@
         <v>12</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1342,10 +1339,10 @@
         <v>39</v>
       </c>
       <c r="B39" s="3" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D39" s="3" t="s">
         <v>10</v>
@@ -1359,16 +1356,16 @@
         <v>40</v>
       </c>
       <c r="B40" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D40" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D40" s="3" t="s">
-        <v>53</v>
-      </c>
       <c r="E40" s="3" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -1376,16 +1373,16 @@
         <v>41</v>
       </c>
       <c r="B41" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="D41" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="D41" s="3" t="s">
+      <c r="E41" s="3" t="s">
         <v>55</v>
-      </c>
-      <c r="E41" s="3" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -1393,16 +1390,16 @@
         <v>42</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1410,16 +1407,16 @@
         <v>43</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D43" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E43" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -1427,16 +1424,16 @@
         <v>44</v>
       </c>
       <c r="B44" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D44" s="3" t="s">
         <v>5</v>
       </c>
       <c r="E44" s="3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -1447,13 +1444,13 @@
         <v>13</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D45" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E45" s="3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -1464,13 +1461,13 @@
         <v>10</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D46" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E46" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -1481,10 +1478,10 @@
         <v>10</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>3</v>
@@ -1495,16 +1492,16 @@
         <v>48</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1512,16 +1509,16 @@
         <v>49</v>
       </c>
       <c r="B49" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E49" s="3" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1529,16 +1526,16 @@
         <v>50</v>
       </c>
       <c r="B50" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D50" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1549,13 +1546,13 @@
         <v>10</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
@@ -1563,16 +1560,16 @@
         <v>52</v>
       </c>
       <c r="B52" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C52" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D52" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E52" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
@@ -1583,13 +1580,13 @@
         <v>10</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E53" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
@@ -1597,16 +1594,16 @@
         <v>54</v>
       </c>
       <c r="B54" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D54" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E54" s="3" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
@@ -1614,16 +1611,16 @@
         <v>55</v>
       </c>
       <c r="B55" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D55" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E55" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
@@ -1631,16 +1628,16 @@
         <v>56</v>
       </c>
       <c r="B56" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D56" s="3" t="s">
         <v>3</v>
       </c>
       <c r="E56" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
@@ -1651,13 +1648,13 @@
         <v>12</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D57" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -1668,13 +1665,13 @@
         <v>18</v>
       </c>
       <c r="C58" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D58" s="3" t="s">
         <v>2</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -1685,10 +1682,10 @@
         <v>3</v>
       </c>
       <c r="C59" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D59" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>5</v>
@@ -1702,7 +1699,7 @@
         <v>22</v>
       </c>
       <c r="C60" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D60" s="3" t="s">
         <v>13</v>
@@ -1719,13 +1716,13 @@
         <v>5</v>
       </c>
       <c r="C61" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D61" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E61" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -1736,13 +1733,13 @@
         <v>14</v>
       </c>
       <c r="C62" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D62" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E62" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -1750,16 +1747,16 @@
         <v>63</v>
       </c>
       <c r="B63" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="C63" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D63" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="C63" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D63" s="3" t="s">
+      <c r="E63" s="3" t="s">
         <v>83</v>
-      </c>
-      <c r="E63" s="3" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -1767,16 +1764,16 @@
         <v>64</v>
       </c>
       <c r="B64" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C64" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D64" s="3" t="s">
         <v>12</v>
       </c>
       <c r="E64" s="3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -1784,16 +1781,16 @@
         <v>65</v>
       </c>
       <c r="B65" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C65" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D65" s="3" t="s">
         <v>11</v>
       </c>
       <c r="E65" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -1801,16 +1798,16 @@
         <v>66</v>
       </c>
       <c r="B66" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="C66" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D66" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="C66" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D66" s="3" t="s">
-        <v>90</v>
-      </c>
       <c r="E66" s="3" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -1821,13 +1818,13 @@
         <v>1</v>
       </c>
       <c r="C67" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D67" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="E67" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="E67" s="3" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -1835,16 +1832,16 @@
         <v>68</v>
       </c>
       <c r="B68" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C68" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D68" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E68" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -1852,16 +1849,16 @@
         <v>69</v>
       </c>
       <c r="B69" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="D69" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="C69" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="D69" s="3" t="s">
+      <c r="E69" s="3" t="s">
         <v>94</v>
-      </c>
-      <c r="E69" s="3" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
@@ -1872,7 +1869,7 @@
         <v>10</v>
       </c>
       <c r="C70" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D70" s="3" t="s">
         <v>10</v>
@@ -1889,7 +1886,7 @@
         <v>19</v>
       </c>
       <c r="C71" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D71" s="3" t="s">
         <v>5</v>
@@ -1906,13 +1903,13 @@
         <v>14</v>
       </c>
       <c r="C72" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D72" s="3" t="s">
         <v>10</v>
       </c>
       <c r="E72" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
@@ -1920,16 +1917,16 @@
         <v>73</v>
       </c>
       <c r="B73" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C73" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D73" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E73" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -1937,16 +1934,16 @@
         <v>74</v>
       </c>
       <c r="B74" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C74" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D74" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E74" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -1954,16 +1951,16 @@
         <v>75</v>
       </c>
       <c r="B75" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C75" s="3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D75" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E75" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
@@ -1971,13 +1968,13 @@
         <v>76</v>
       </c>
       <c r="B76" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C76" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D76" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E76" s="3" t="s">
         <v>18</v>
@@ -1991,7 +1988,7 @@
         <v>6</v>
       </c>
       <c r="C77" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D77" s="3" t="s">
         <v>3</v>
@@ -2008,7 +2005,7 @@
         <v>19</v>
       </c>
       <c r="C78" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D78" s="3" t="s">
         <v>3</v>
@@ -2022,13 +2019,13 @@
         <v>79</v>
       </c>
       <c r="B79" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C79" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>18</v>
@@ -2039,16 +2036,16 @@
         <v>80</v>
       </c>
       <c r="B80" s="3" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C80" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D80" s="3" t="s">
         <v>20</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
@@ -2059,13 +2056,13 @@
         <v>22</v>
       </c>
       <c r="C81" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D81" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E81" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2073,16 +2070,16 @@
         <v>82</v>
       </c>
       <c r="B82" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C82" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D82" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -2090,16 +2087,16 @@
         <v>83</v>
       </c>
       <c r="B83" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C83" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D83" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
@@ -2107,16 +2104,16 @@
         <v>84</v>
       </c>
       <c r="B84" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C84" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D84" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E84" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
@@ -2127,13 +2124,13 @@
         <v>20</v>
       </c>
       <c r="C85" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D85" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E85" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.25">
@@ -2141,16 +2138,16 @@
         <v>86</v>
       </c>
       <c r="B86" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C86" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D86" s="3" t="s">
         <v>19</v>
       </c>
       <c r="E86" s="3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.25">
@@ -2161,13 +2158,13 @@
         <v>19</v>
       </c>
       <c r="C87" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E87" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.25">
@@ -2178,7 +2175,7 @@
         <v>18</v>
       </c>
       <c r="C88" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D88" s="3" t="s">
         <v>12</v>
@@ -2195,13 +2192,13 @@
         <v>10</v>
       </c>
       <c r="C89" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D89" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E89" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.25">
@@ -2209,16 +2206,16 @@
         <v>90</v>
       </c>
       <c r="B90" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C90" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D90" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E90" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.25">
@@ -2229,7 +2226,7 @@
         <v>10</v>
       </c>
       <c r="C91" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D91" s="3" t="s">
         <v>13</v>
@@ -2243,16 +2240,16 @@
         <v>92</v>
       </c>
       <c r="B92" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C92" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D92" s="3" t="s">
         <v>14</v>
       </c>
       <c r="E92" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -2260,16 +2257,16 @@
         <v>93</v>
       </c>
       <c r="B93" s="3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C93" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E93" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -2277,16 +2274,16 @@
         <v>94</v>
       </c>
       <c r="B94" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C94" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E94" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.25">
@@ -2294,16 +2291,16 @@
         <v>95</v>
       </c>
       <c r="B95" s="3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C95" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D95" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="E95" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
@@ -2314,13 +2311,13 @@
         <v>11</v>
       </c>
       <c r="C96" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D96" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E96" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
@@ -2328,16 +2325,16 @@
         <v>97</v>
       </c>
       <c r="B97" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C97" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D97" s="3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E97" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -2348,13 +2345,13 @@
         <v>11</v>
       </c>
       <c r="C98" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D98" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="E98" s="3" t="s">
         <v>105</v>
-      </c>
-      <c r="E98" s="3" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -2365,13 +2362,13 @@
         <v>11</v>
       </c>
       <c r="C99" s="3" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D99" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E99" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>